<commit_message>
fix: app.py red stuff and no info found bug
</commit_message>
<xml_diff>
--- a/given_files/Production_Electrolysis_Occupations.xlsx
+++ b/given_files/Production_Electrolysis_Occupations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udwinprod-my.sharepoint.com/personal/bika_udel_edu/Documents/Desktop/WF Jobs Skills Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli Brignac\OneDrive\Desktop\Hydrogen\MACH-2-Hydrogen-Hub\given_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="420" documentId="8_{5814F701-1DC0-4321-BD94-F3DCF09F31F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71E77F2F-F916-4BEF-98A9-66319A8279FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7268B11D-5628-4703-B04E-4F93A5B22355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jobs" sheetId="5" r:id="rId1"/>
@@ -4706,7 +4706,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5156,21 +5156,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B132BA85-1248-4B90-8529-1C705C7DADC1}">
   <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124:C131"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="255.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="255.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>2001</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2001</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2001</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>2001</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>2001</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>2001</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>2001</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>2001</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>2001</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>2001</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>2001</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>2001</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>2001</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>2001</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>2001</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>2001</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>2001</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>2001</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>2001</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>2001</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>3001</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>3001</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>3001</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>3001</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>3001</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>3001</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>3001</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>3001</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>3001</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>3001</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>3001</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>3001</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>3001</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>3002</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>3002</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>3002</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>3002</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>3002</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>4001</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>4001</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>4001</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>4001</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>4001</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>4001</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>4001</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>4001</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>4002</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>4002</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>4002</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>4002</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>4002</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>4002</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>4002</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>4002</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>4002</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>4002</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>4002</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>4002</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>4002</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>4002</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>4002</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>4003</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>4003</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>4003</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>4003</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>4003</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>4003</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>4003</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>4003</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>4003</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>4004</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>4004</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>4004</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>4004</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>4004</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>4004</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>4004</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>4004</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>4004</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>4004</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>4004</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>4004</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>4004</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>4004</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>4004</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>4004</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>4004</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>1001</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>1001</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>1001</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>1001</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>1001</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>1001</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>1001</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>1001</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>1001</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>1001</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>1001</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>1001</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>1001</v>
       </c>
@@ -7796,7 +7796,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>1001</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>1001</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>1001</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>1001</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>1001</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>1001</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>1001</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>1001</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>1001</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>5001</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>5002</v>
       </c>
@@ -8082,7 +8082,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>5002</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>5002</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>5002</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>5002</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>5003</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>5003</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>5003</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>5003</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>5003</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>5003</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>5003</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>5004</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>5004</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>5004</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>5004</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>5004</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>5004</v>
       </c>
@@ -8524,7 +8524,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>5004</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>5004</v>
       </c>
@@ -8589,15 +8589,15 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>598</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>599</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>600</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>602</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>603</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>604</v>
       </c>
@@ -8681,7 +8681,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>605</v>
       </c>
@@ -8695,7 +8695,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>606</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>607</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>609</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>610</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>605</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>611</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>613</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>615</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>616</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>617</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>618</v>
       </c>
@@ -8865,14 +8865,14 @@
       <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>404</v>
       </c>
@@ -8894,7 +8894,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>601</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -8916,7 +8916,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>188</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>188</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>188</v>
       </c>
@@ -8960,7 +8960,7 @@
         <v>4003</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>188</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>492</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>5001</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>492</v>
       </c>
@@ -8993,7 +8993,7 @@
         <v>5002</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>492</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>5003</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>492</v>
       </c>
@@ -9021,21 +9021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100253C3D666B5A6743BA6EB287623FC2FB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6913fe596d975c314c9f80c663f2a144">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96af757-959e-46a2-a2e6-5d37bd3bf925" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6320560504c0e12024addc45626da4d1" ns2:_="">
     <xsd:import namespace="c96af757-959e-46a2-a2e6-5d37bd3bf925"/>
@@ -9179,14 +9164,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260C0077-AE67-4B5B-8016-F1839C7ABD73}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCB1609-E0C9-4B53-BC76-C8EC3C68A9A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c96af757-959e-46a2-a2e6-5d37bd3bf925"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8D3927B-A508-49B4-A5E9-9DD93B7B43E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8D3927B-A508-49B4-A5E9-9DD93B7B43E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CCB1609-E0C9-4B53-BC76-C8EC3C68A9A3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260C0077-AE67-4B5B-8016-F1839C7ABD73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>